<commit_message>
Added TrackOrder page implementation and deleted Admincommonbase class
</commit_message>
<xml_diff>
--- a/bin/testdata/regTestdata.xlsx
+++ b/bin/testdata/regTestdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivam_kushwaha\eclipse-workspace\ShoppingPortal\src\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9745C8-DE14-49DF-897A-77DF30DBA82C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CCA249-58C8-424A-9195-5BBB61BAFFCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CC31A2FF-7F59-4B39-8234-9CDEA7BCDCFF}"/>
+    <workbookView xWindow="2540" yWindow="2540" windowWidth="14400" windowHeight="7360" xr2:uid="{CC31A2FF-7F59-4B39-8234-9CDEA7BCDCFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,13 +81,13 @@
     <t>You are successfully register</t>
   </si>
   <si>
-    <t>fake4</t>
-  </si>
-  <si>
-    <t>fake4@g.com</t>
-  </si>
-  <si>
-    <t>fake@1234</t>
+    <t>fake5</t>
+  </si>
+  <si>
+    <t>fake5@g.com</t>
+  </si>
+  <si>
+    <t>fake@12345</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,7 +529,7 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>987654321</v>
+        <v>987654341</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>

</xml_diff>